<commit_message>
HNRS-1 changed dietary assessment category in DPE
</commit_message>
<xml_diff>
--- a/analyst/Franzi/rmonize/data_proc_elem/DPE_HNRS_FRANZI.xlsx
+++ b/analyst/Franzi/rmonize/data_proc_elem/DPE_HNRS_FRANZI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\analyst\Franzi\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A9F956-B2BB-44C5-B13C-A9270C167AE6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{BB16497B-FF54-4F8C-B89B-CEC5DE1AE4AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -886,9 +886,6 @@
     <t>paste</t>
   </si>
   <si>
-    <t>1(FFQ)</t>
-  </si>
-  <si>
     <t>complete</t>
   </si>
   <si>
@@ -972,6 +969,9 @@
   </si>
   <si>
     <t>includes only whole grain bread and black bread</t>
+  </si>
+  <si>
+    <t>0(FPQ)</t>
   </si>
 </sst>
 </file>
@@ -1407,24 +1407,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F119" sqref="F119"/>
+    <sheetView tabSelected="1" topLeftCell="B109" workbookViewId="0">
+      <selection activeCell="H127" sqref="H127"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -1470,16 +1470,16 @@
         <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G2" t="s">
         <v>253</v>
       </c>
       <c r="H2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I2" t="s">
         <v>254</v>
@@ -1491,7 +1491,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -1502,19 +1502,19 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G3" t="s">
         <v>253</v>
       </c>
       <c r="H3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J3" t="s">
         <v>255</v>
@@ -1523,7 +1523,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>16</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>257</v>
@@ -1552,7 +1552,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>18</v>
       </c>
@@ -1563,19 +1563,19 @@
         <v>13</v>
       </c>
       <c r="E5" t="s">
+        <v>292</v>
+      </c>
+      <c r="F5" t="s">
         <v>293</v>
-      </c>
-      <c r="F5" t="s">
-        <v>294</v>
       </c>
       <c r="G5" t="s">
         <v>253</v>
       </c>
       <c r="H5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J5" t="s">
         <v>255</v>
@@ -1584,7 +1584,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>20</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>257</v>
@@ -1613,7 +1613,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>22</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>257</v>
@@ -1642,7 +1642,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>24</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>257</v>
@@ -1671,7 +1671,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>26</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>257</v>
@@ -1700,7 +1700,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>28</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>257</v>
@@ -1729,7 +1729,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>30</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>257</v>
@@ -1758,7 +1758,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>32</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>13</v>
       </c>
       <c r="E12" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>257</v>
@@ -1787,7 +1787,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>34</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>257</v>
@@ -1816,7 +1816,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>36</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>257</v>
@@ -1845,7 +1845,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>38</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>257</v>
@@ -1874,7 +1874,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>40</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>13</v>
       </c>
       <c r="E16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>257</v>
@@ -1903,7 +1903,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>42</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>13</v>
       </c>
       <c r="E17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>259</v>
@@ -1926,7 +1926,7 @@
         <v>260</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>255</v>
@@ -1935,7 +1935,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>44</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>13</v>
       </c>
       <c r="E18" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>257</v>
@@ -1964,7 +1964,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>46</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>13</v>
       </c>
       <c r="E19" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>257</v>
@@ -1993,7 +1993,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>48</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>13</v>
       </c>
       <c r="E20" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>257</v>
@@ -2022,7 +2022,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>50</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>13</v>
       </c>
       <c r="E21" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>257</v>
@@ -2051,7 +2051,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>52</v>
       </c>
@@ -2062,19 +2062,19 @@
         <v>13</v>
       </c>
       <c r="E22" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>253</v>
       </c>
       <c r="H22" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="I22" s="5" t="s">
         <v>297</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>298</v>
       </c>
       <c r="J22" s="5" t="s">
         <v>255</v>
@@ -2083,7 +2083,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>54</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>13</v>
       </c>
       <c r="E23" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>261</v>
@@ -2106,7 +2106,7 @@
         <v>260</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>255</v>
@@ -2115,7 +2115,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>56</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>13</v>
       </c>
       <c r="E24" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>257</v>
@@ -2144,7 +2144,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="25" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>58</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>13</v>
       </c>
       <c r="E25" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>262</v>
@@ -2164,10 +2164,10 @@
         <v>253</v>
       </c>
       <c r="H25" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="I25" s="8" t="s">
         <v>299</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>300</v>
       </c>
       <c r="J25" s="5" t="s">
         <v>255</v>
@@ -2176,7 +2176,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="26" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>60</v>
       </c>
@@ -2187,7 +2187,7 @@
         <v>13</v>
       </c>
       <c r="E26" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>262</v>
@@ -2196,10 +2196,10 @@
         <v>253</v>
       </c>
       <c r="H26" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="I26" s="8" t="s">
         <v>299</v>
-      </c>
-      <c r="I26" s="8" t="s">
-        <v>300</v>
       </c>
       <c r="J26" s="5" t="s">
         <v>255</v>
@@ -2208,7 +2208,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>62</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>13</v>
       </c>
       <c r="E27" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>263</v>
@@ -2231,7 +2231,7 @@
         <v>260</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J27" s="5" t="s">
         <v>255</v>
@@ -2240,7 +2240,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>64</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>13</v>
       </c>
       <c r="E28" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>257</v>
@@ -2269,7 +2269,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>66</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>13</v>
       </c>
       <c r="E29" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>257</v>
@@ -2298,7 +2298,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>68</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>13</v>
       </c>
       <c r="E30" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>257</v>
@@ -2327,7 +2327,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>70</v>
       </c>
@@ -2338,7 +2338,7 @@
         <v>13</v>
       </c>
       <c r="E31" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>257</v>
@@ -2356,7 +2356,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>72</v>
       </c>
@@ -2367,7 +2367,7 @@
         <v>13</v>
       </c>
       <c r="E32" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>257</v>
@@ -2385,7 +2385,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>74</v>
       </c>
@@ -2396,19 +2396,19 @@
         <v>13</v>
       </c>
       <c r="E33" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>253</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J33" s="5" t="s">
         <v>255</v>
@@ -2417,7 +2417,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>76</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>13</v>
       </c>
       <c r="E34" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>257</v>
@@ -2446,7 +2446,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>78</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>13</v>
       </c>
       <c r="E35" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>265</v>
@@ -2469,7 +2469,7 @@
         <v>260</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J35" s="5" t="s">
         <v>255</v>
@@ -2478,7 +2478,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="36" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>80</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>13</v>
       </c>
       <c r="E36" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>266</v>
@@ -2501,7 +2501,7 @@
         <v>260</v>
       </c>
       <c r="I36" s="10" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J36" s="5" t="s">
         <v>255</v>
@@ -2510,7 +2510,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>82</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>13</v>
       </c>
       <c r="E37" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>257</v>
@@ -2539,7 +2539,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>84</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>13</v>
       </c>
       <c r="E38" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>257</v>
@@ -2568,7 +2568,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>86</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>13</v>
       </c>
       <c r="E39" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>264</v>
@@ -2591,7 +2591,7 @@
         <v>260</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J39" s="3" t="s">
         <v>255</v>
@@ -2600,7 +2600,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>88</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>13</v>
       </c>
       <c r="E40" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>257</v>
@@ -2629,7 +2629,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>90</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>13</v>
       </c>
       <c r="E41" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>257</v>
@@ -2658,7 +2658,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>92</v>
       </c>
@@ -2669,28 +2669,28 @@
         <v>13</v>
       </c>
       <c r="E42" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>253</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J42" s="5" t="s">
         <v>255</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>94</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>13</v>
       </c>
       <c r="E43" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F43" s="4" t="s">
         <v>267</v>
@@ -2713,7 +2713,7 @@
         <v>260</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J43" s="5" t="s">
         <v>255</v>
@@ -2722,7 +2722,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>96</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>13</v>
       </c>
       <c r="E44" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>257</v>
@@ -2751,7 +2751,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>98</v>
       </c>
@@ -2762,7 +2762,7 @@
         <v>13</v>
       </c>
       <c r="E45" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>257</v>
@@ -2780,7 +2780,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>100</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>13</v>
       </c>
       <c r="E46" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>257</v>
@@ -2809,7 +2809,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>102</v>
       </c>
@@ -2820,7 +2820,7 @@
         <v>13</v>
       </c>
       <c r="E47" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>257</v>
@@ -2838,7 +2838,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>104</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>13</v>
       </c>
       <c r="E48" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>257</v>
@@ -2867,7 +2867,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>106</v>
       </c>
@@ -2878,7 +2878,7 @@
         <v>13</v>
       </c>
       <c r="E49" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>257</v>
@@ -2896,7 +2896,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>108</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>13</v>
       </c>
       <c r="E50" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F50" s="4" t="s">
         <v>268</v>
@@ -2919,7 +2919,7 @@
         <v>260</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J50" s="5" t="s">
         <v>255</v>
@@ -2928,7 +2928,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>110</v>
       </c>
@@ -2939,7 +2939,7 @@
         <v>13</v>
       </c>
       <c r="E51" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>257</v>
@@ -2957,7 +2957,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>112</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>13</v>
       </c>
       <c r="E52" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>257</v>
@@ -2986,7 +2986,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>114</v>
       </c>
@@ -2997,7 +2997,7 @@
         <v>13</v>
       </c>
       <c r="E53" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>257</v>
@@ -3015,7 +3015,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>116</v>
       </c>
@@ -3026,7 +3026,7 @@
         <v>13</v>
       </c>
       <c r="E54" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>257</v>
@@ -3044,7 +3044,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>118</v>
       </c>
@@ -3055,7 +3055,7 @@
         <v>13</v>
       </c>
       <c r="E55" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>257</v>
@@ -3073,7 +3073,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>120</v>
       </c>
@@ -3084,7 +3084,7 @@
         <v>13</v>
       </c>
       <c r="E56" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>257</v>
@@ -3102,7 +3102,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>122</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>13</v>
       </c>
       <c r="E57" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>257</v>
@@ -3131,7 +3131,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>124</v>
       </c>
@@ -3142,28 +3142,28 @@
         <v>13</v>
       </c>
       <c r="E58" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>253</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J58" s="5" t="s">
         <v>255</v>
       </c>
       <c r="K58" s="5" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.3">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>126</v>
       </c>
@@ -3174,7 +3174,7 @@
         <v>13</v>
       </c>
       <c r="E59" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F59" s="5" t="s">
         <v>257</v>
@@ -3192,7 +3192,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>128</v>
       </c>
@@ -3203,7 +3203,7 @@
         <v>13</v>
       </c>
       <c r="E60" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F60" s="4" t="s">
         <v>269</v>
@@ -3215,7 +3215,7 @@
         <v>260</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J60" s="5" t="s">
         <v>255</v>
@@ -3224,7 +3224,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>130</v>
       </c>
@@ -3235,7 +3235,7 @@
         <v>13</v>
       </c>
       <c r="E61" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>257</v>
@@ -3253,7 +3253,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>132</v>
       </c>
@@ -3264,7 +3264,7 @@
         <v>13</v>
       </c>
       <c r="E62" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F62" s="5" t="s">
         <v>257</v>
@@ -3282,7 +3282,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>134</v>
       </c>
@@ -3293,7 +3293,7 @@
         <v>13</v>
       </c>
       <c r="E63" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>257</v>
@@ -3311,7 +3311,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>136</v>
       </c>
@@ -3322,7 +3322,7 @@
         <v>13</v>
       </c>
       <c r="E64" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F64" s="4" t="s">
         <v>270</v>
@@ -3334,7 +3334,7 @@
         <v>260</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J64" s="5" t="s">
         <v>255</v>
@@ -3343,7 +3343,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>138</v>
       </c>
@@ -3354,7 +3354,7 @@
         <v>13</v>
       </c>
       <c r="E65" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F65" s="5" t="s">
         <v>257</v>
@@ -3372,7 +3372,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>140</v>
       </c>
@@ -3383,19 +3383,19 @@
         <v>13</v>
       </c>
       <c r="E66" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G66" s="5" t="s">
         <v>253</v>
       </c>
       <c r="H66" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I66" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J66" s="5" t="s">
         <v>255</v>
@@ -3404,7 +3404,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>142</v>
       </c>
@@ -3415,19 +3415,19 @@
         <v>13</v>
       </c>
       <c r="E67" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F67" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G67" s="5" t="s">
         <v>253</v>
       </c>
       <c r="H67" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I67" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J67" s="3" t="s">
         <v>255</v>
@@ -3436,7 +3436,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>144</v>
       </c>
@@ -3447,7 +3447,7 @@
         <v>13</v>
       </c>
       <c r="E68" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F68" s="4" t="s">
         <v>271</v>
@@ -3459,7 +3459,7 @@
         <v>260</v>
       </c>
       <c r="I68" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J68" s="5" t="s">
         <v>255</v>
@@ -3468,7 +3468,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>146</v>
       </c>
@@ -3479,7 +3479,7 @@
         <v>13</v>
       </c>
       <c r="E69" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F69" s="4" t="s">
         <v>272</v>
@@ -3491,7 +3491,7 @@
         <v>260</v>
       </c>
       <c r="I69" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J69" s="5" t="s">
         <v>255</v>
@@ -3500,7 +3500,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>148</v>
       </c>
@@ -3511,7 +3511,7 @@
         <v>13</v>
       </c>
       <c r="E70" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F70" s="5" t="s">
         <v>257</v>
@@ -3529,7 +3529,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>150</v>
       </c>
@@ -3540,7 +3540,7 @@
         <v>13</v>
       </c>
       <c r="E71" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F71" s="5" t="s">
         <v>257</v>
@@ -3558,7 +3558,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>152</v>
       </c>
@@ -3569,7 +3569,7 @@
         <v>13</v>
       </c>
       <c r="E72" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F72" s="4" t="s">
         <v>273</v>
@@ -3581,7 +3581,7 @@
         <v>260</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J72" s="5" t="s">
         <v>255</v>
@@ -3590,7 +3590,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>154</v>
       </c>
@@ -3601,7 +3601,7 @@
         <v>13</v>
       </c>
       <c r="E73" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F73" s="4" t="s">
         <v>274</v>
@@ -3613,7 +3613,7 @@
         <v>260</v>
       </c>
       <c r="I73" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J73" s="3" t="s">
         <v>255</v>
@@ -3622,7 +3622,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>156</v>
       </c>
@@ -3633,7 +3633,7 @@
         <v>13</v>
       </c>
       <c r="E74" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F74" s="5" t="s">
         <v>257</v>
@@ -3651,7 +3651,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>158</v>
       </c>
@@ -3662,7 +3662,7 @@
         <v>13</v>
       </c>
       <c r="E75" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F75" s="5" t="s">
         <v>257</v>
@@ -3680,7 +3680,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>160</v>
       </c>
@@ -3691,7 +3691,7 @@
         <v>13</v>
       </c>
       <c r="E76" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F76" s="5" t="s">
         <v>257</v>
@@ -3709,7 +3709,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>162</v>
       </c>
@@ -3720,7 +3720,7 @@
         <v>13</v>
       </c>
       <c r="E77" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F77" s="5" t="s">
         <v>257</v>
@@ -3738,7 +3738,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>164</v>
       </c>
@@ -3749,7 +3749,7 @@
         <v>13</v>
       </c>
       <c r="E78" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F78" s="5" t="s">
         <v>257</v>
@@ -3767,7 +3767,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>166</v>
       </c>
@@ -3778,7 +3778,7 @@
         <v>13</v>
       </c>
       <c r="E79" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F79" s="5" t="s">
         <v>257</v>
@@ -3796,7 +3796,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>168</v>
       </c>
@@ -3807,7 +3807,7 @@
         <v>13</v>
       </c>
       <c r="E80" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F80" s="5" t="s">
         <v>257</v>
@@ -3825,7 +3825,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>170</v>
       </c>
@@ -3836,7 +3836,7 @@
         <v>13</v>
       </c>
       <c r="E81" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F81" s="5" t="s">
         <v>257</v>
@@ -3854,7 +3854,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="82" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>172</v>
       </c>
@@ -3865,7 +3865,7 @@
         <v>13</v>
       </c>
       <c r="E82" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F82" s="5" t="s">
         <v>257</v>
@@ -3883,7 +3883,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="83" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>174</v>
       </c>
@@ -3894,7 +3894,7 @@
         <v>13</v>
       </c>
       <c r="E83" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F83" s="5" t="s">
         <v>257</v>
@@ -3912,7 +3912,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="84" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>176</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>13</v>
       </c>
       <c r="E84" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F84" s="5" t="s">
         <v>257</v>
@@ -3941,7 +3941,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="85" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>178</v>
       </c>
@@ -3952,28 +3952,28 @@
         <v>13</v>
       </c>
       <c r="E85" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G85" s="5" t="s">
         <v>253</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I85" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J85" s="5" t="s">
         <v>255</v>
       </c>
       <c r="K85" s="5" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="86" spans="2:11" x14ac:dyDescent="0.3">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="86" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>180</v>
       </c>
@@ -3984,7 +3984,7 @@
         <v>13</v>
       </c>
       <c r="E86" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F86" s="4" t="s">
         <v>275</v>
@@ -3996,7 +3996,7 @@
         <v>260</v>
       </c>
       <c r="I86" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J86" s="5" t="s">
         <v>255</v>
@@ -4005,7 +4005,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="87" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>182</v>
       </c>
@@ -4016,7 +4016,7 @@
         <v>13</v>
       </c>
       <c r="E87" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F87" s="4" t="s">
         <v>276</v>
@@ -4028,7 +4028,7 @@
         <v>260</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J87" s="5" t="s">
         <v>255</v>
@@ -4037,7 +4037,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="88" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>184</v>
       </c>
@@ -4048,28 +4048,28 @@
         <v>13</v>
       </c>
       <c r="E88" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G88" s="5" t="s">
         <v>253</v>
       </c>
       <c r="H88" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I88" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J88" s="5" t="s">
         <v>255</v>
       </c>
       <c r="K88" s="5" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="89" spans="2:11" x14ac:dyDescent="0.3">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="89" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>186</v>
       </c>
@@ -4080,7 +4080,7 @@
         <v>13</v>
       </c>
       <c r="E89" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F89" s="4" t="s">
         <v>277</v>
@@ -4092,7 +4092,7 @@
         <v>260</v>
       </c>
       <c r="I89" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J89" s="5" t="s">
         <v>255</v>
@@ -4101,7 +4101,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="90" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>188</v>
       </c>
@@ -4112,7 +4112,7 @@
         <v>13</v>
       </c>
       <c r="E90" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F90" s="4" t="s">
         <v>278</v>
@@ -4124,7 +4124,7 @@
         <v>260</v>
       </c>
       <c r="I90" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J90" s="5" t="s">
         <v>255</v>
@@ -4133,7 +4133,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="91" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>190</v>
       </c>
@@ -4144,7 +4144,7 @@
         <v>13</v>
       </c>
       <c r="E91" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F91" s="4" t="s">
         <v>279</v>
@@ -4156,7 +4156,7 @@
         <v>260</v>
       </c>
       <c r="I91" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J91" s="5" t="s">
         <v>255</v>
@@ -4165,7 +4165,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="92" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>192</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>13</v>
       </c>
       <c r="E92" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F92" s="5" t="s">
         <v>257</v>
@@ -4194,7 +4194,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="93" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>194</v>
       </c>
@@ -4205,7 +4205,7 @@
         <v>13</v>
       </c>
       <c r="E93" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F93" s="4" t="s">
         <v>280</v>
@@ -4217,7 +4217,7 @@
         <v>260</v>
       </c>
       <c r="I93" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J93" s="5" t="s">
         <v>255</v>
@@ -4226,7 +4226,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="94" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>196</v>
       </c>
@@ -4237,7 +4237,7 @@
         <v>13</v>
       </c>
       <c r="E94" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F94" s="4" t="s">
         <v>281</v>
@@ -4249,7 +4249,7 @@
         <v>260</v>
       </c>
       <c r="I94" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J94" s="5" t="s">
         <v>255</v>
@@ -4258,7 +4258,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="95" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>198</v>
       </c>
@@ -4269,7 +4269,7 @@
         <v>13</v>
       </c>
       <c r="E95" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F95" s="4" t="s">
         <v>282</v>
@@ -4281,7 +4281,7 @@
         <v>260</v>
       </c>
       <c r="I95" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J95" s="5" t="s">
         <v>255</v>
@@ -4290,7 +4290,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="96" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>200</v>
       </c>
@@ -4301,7 +4301,7 @@
         <v>13</v>
       </c>
       <c r="E96" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F96" s="5" t="s">
         <v>257</v>
@@ -4319,7 +4319,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="97" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>202</v>
       </c>
@@ -4330,7 +4330,7 @@
         <v>13</v>
       </c>
       <c r="E97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F97" s="4" t="s">
         <v>283</v>
@@ -4342,7 +4342,7 @@
         <v>260</v>
       </c>
       <c r="I97" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J97" s="5" t="s">
         <v>255</v>
@@ -4351,7 +4351,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="98" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>204</v>
       </c>
@@ -4362,7 +4362,7 @@
         <v>13</v>
       </c>
       <c r="E98" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F98" s="4" t="s">
         <v>284</v>
@@ -4374,7 +4374,7 @@
         <v>260</v>
       </c>
       <c r="I98" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J98" s="5" t="s">
         <v>255</v>
@@ -4383,7 +4383,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="99" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>206</v>
       </c>
@@ -4394,7 +4394,7 @@
         <v>13</v>
       </c>
       <c r="E99" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F99" s="5" t="s">
         <v>257</v>
@@ -4412,7 +4412,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="100" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>208</v>
       </c>
@@ -4423,7 +4423,7 @@
         <v>13</v>
       </c>
       <c r="E100" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F100" s="5" t="s">
         <v>257</v>
@@ -4441,7 +4441,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="101" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>210</v>
       </c>
@@ -4452,7 +4452,7 @@
         <v>13</v>
       </c>
       <c r="E101" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F101" s="5" t="s">
         <v>257</v>
@@ -4470,7 +4470,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="102" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>212</v>
       </c>
@@ -4481,7 +4481,7 @@
         <v>13</v>
       </c>
       <c r="E102" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F102" s="5" t="s">
         <v>257</v>
@@ -4499,7 +4499,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="103" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>214</v>
       </c>
@@ -4510,7 +4510,7 @@
         <v>13</v>
       </c>
       <c r="E103" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F103" s="5" t="s">
         <v>257</v>
@@ -4528,7 +4528,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="104" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>216</v>
       </c>
@@ -4539,7 +4539,7 @@
         <v>13</v>
       </c>
       <c r="E104" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F104" s="5" t="s">
         <v>257</v>
@@ -4557,7 +4557,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="105" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>218</v>
       </c>
@@ -4568,7 +4568,7 @@
         <v>13</v>
       </c>
       <c r="E105" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F105" s="5" t="s">
         <v>257</v>
@@ -4586,7 +4586,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="106" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>220</v>
       </c>
@@ -4597,7 +4597,7 @@
         <v>13</v>
       </c>
       <c r="E106" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F106" s="5" t="s">
         <v>257</v>
@@ -4615,7 +4615,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="107" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>222</v>
       </c>
@@ -4626,7 +4626,7 @@
         <v>13</v>
       </c>
       <c r="E107" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F107" s="5" t="s">
         <v>257</v>
@@ -4644,7 +4644,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="108" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>224</v>
       </c>
@@ -4655,7 +4655,7 @@
         <v>13</v>
       </c>
       <c r="E108" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F108" s="5" t="s">
         <v>257</v>
@@ -4673,7 +4673,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="109" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>226</v>
       </c>
@@ -4684,7 +4684,7 @@
         <v>13</v>
       </c>
       <c r="E109" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F109" s="5" t="s">
         <v>257</v>
@@ -4702,7 +4702,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="110" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>228</v>
       </c>
@@ -4713,7 +4713,7 @@
         <v>13</v>
       </c>
       <c r="E110" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F110" s="5" t="s">
         <v>257</v>
@@ -4731,7 +4731,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="111" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>230</v>
       </c>
@@ -4742,7 +4742,7 @@
         <v>13</v>
       </c>
       <c r="E111" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F111" s="5" t="s">
         <v>257</v>
@@ -4760,7 +4760,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="112" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>232</v>
       </c>
@@ -4771,7 +4771,7 @@
         <v>13</v>
       </c>
       <c r="E112" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F112" s="5" t="s">
         <v>257</v>
@@ -4789,7 +4789,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="113" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>234</v>
       </c>
@@ -4800,7 +4800,7 @@
         <v>13</v>
       </c>
       <c r="E113" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F113" s="5" t="s">
         <v>257</v>
@@ -4818,7 +4818,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="114" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>236</v>
       </c>
@@ -4829,7 +4829,7 @@
         <v>13</v>
       </c>
       <c r="E114" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F114" s="5" t="s">
         <v>257</v>
@@ -4847,7 +4847,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="115" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>238</v>
       </c>
@@ -4858,7 +4858,7 @@
         <v>13</v>
       </c>
       <c r="E115" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F115" s="5" t="s">
         <v>257</v>
@@ -4876,7 +4876,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="116" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>240</v>
       </c>
@@ -4887,7 +4887,7 @@
         <v>13</v>
       </c>
       <c r="E116" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F116" s="5" t="s">
         <v>257</v>
@@ -4905,7 +4905,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="117" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>242</v>
       </c>
@@ -4916,7 +4916,7 @@
         <v>13</v>
       </c>
       <c r="E117" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F117" s="5" t="s">
         <v>257</v>
@@ -4934,7 +4934,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="118" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>244</v>
       </c>
@@ -4945,7 +4945,7 @@
         <v>13</v>
       </c>
       <c r="E118" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F118" s="5" t="s">
         <v>257</v>
@@ -4963,7 +4963,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="119" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>246</v>
       </c>
@@ -4974,7 +4974,7 @@
         <v>13</v>
       </c>
       <c r="E119" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F119" s="4" t="s">
         <v>285</v>
@@ -4986,7 +4986,7 @@
         <v>260</v>
       </c>
       <c r="I119" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J119" s="5" t="s">
         <v>255</v>
@@ -4995,7 +4995,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="120" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>248</v>
       </c>
@@ -5006,7 +5006,7 @@
         <v>13</v>
       </c>
       <c r="E120" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F120" s="5" t="s">
         <v>257</v>
@@ -5024,7 +5024,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="121" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>250</v>
       </c>
@@ -5035,7 +5035,7 @@
         <v>252</v>
       </c>
       <c r="E121" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F121" s="4" t="s">
         <v>286</v>
@@ -5044,16 +5044,16 @@
         <v>287</v>
       </c>
       <c r="H121" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I121" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="J121" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="J121" s="4" t="s">
+      <c r="K121" s="4" t="s">
         <v>289</v>
-      </c>
-      <c r="K121" s="4" t="s">
-        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>